<commit_message>
Ajustes por fase de pruebas de Usuario
</commit_message>
<xml_diff>
--- a/FASE_2_SPRINT_6/PRUEBAS_TECNICAS/Porcentaje_Responsabilidad.xlsx
+++ b/FASE_2_SPRINT_6/PRUEBAS_TECNICAS/Porcentaje_Responsabilidad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Escenario 1</t>
   </si>
@@ -53,13 +53,22 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Fiso1012</t>
-  </si>
-  <si>
     <t>Tipo Garantía Fiduciaria, Tipo Garantía Valor, Tipo Garantía Real, Tipo Garantía Fideicomiso y Tipo Garantía Aval</t>
   </si>
   <si>
     <t>Real123456</t>
+  </si>
+  <si>
+    <t>Tipo Garantía Valor, Tipo Garantía Real, Tipo Garantía Fideicomiso y Tipo Garantía Aval</t>
+  </si>
+  <si>
+    <t>500-02-02-0900796</t>
+  </si>
+  <si>
+    <t>500-02-02-5761941</t>
+  </si>
+  <si>
+    <t>Real-142280</t>
   </si>
 </sst>
 </file>
@@ -277,7 +286,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,41 +298,41 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,14 +346,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,6 +372,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -691,111 +703,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="8">
+      <c r="B5" s="10"/>
+      <c r="C5" s="13">
         <v>55000000</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>19000000</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="13"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="13"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -804,6 +816,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:D4"/>
@@ -820,8 +834,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -833,7 +845,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +853,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
@@ -850,123 +862,121 @@
       <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="A2" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="8">
-        <v>55000000</v>
-      </c>
-      <c r="D5" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="13">
+        <v>14450541.550000001</v>
+      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="5">
         <f>(C5/$C$8)*100</f>
-        <v>60.439560439560438</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="17">
-        <v>19000000</v>
-      </c>
-      <c r="H5" s="18"/>
+        <v>67.115284909424261</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="8">
-        <v>13000000</v>
-      </c>
-      <c r="D6" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="13">
+        <v>7080383.29</v>
+      </c>
+      <c r="D6" s="13"/>
       <c r="E6" s="5">
         <f>(C6/$C$8)*100</f>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
+        <v>32.884715090575739</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="8">
-        <v>23000000</v>
-      </c>
-      <c r="D7" s="8"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="5">
         <f>(C7/$C$8)*100</f>
-        <v>25.274725274725274</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18">
         <f>SUM(C5:D7)</f>
-        <v>91000000</v>
-      </c>
-      <c r="D8" s="25"/>
+        <v>21530924.84</v>
+      </c>
+      <c r="D8" s="18"/>
       <c r="E8" s="6">
         <f>SUM(E5:E7)</f>
-        <v>99.999999999999986</v>
+        <v>100</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20"/>
@@ -976,70 +986,70 @@
       <c r="A9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="8">
+      <c r="B9" s="10"/>
+      <c r="C9" s="13">
         <v>55000000</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="5">
         <f>(C9/$C$8)*100</f>
-        <v>60.439560439560438</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="17">
+        <v>255.44652823190108</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="24">
         <v>58500000</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="8">
+      <c r="B10" s="10"/>
+      <c r="C10" s="13">
         <v>13000000</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="5">
         <f>(C10/$C$8)*100</f>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
+        <v>60.378270309358442</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="8">
+      <c r="B11" s="10"/>
+      <c r="C11" s="13">
         <v>23000000</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="5">
         <f>(C11/$C$8)*100</f>
-        <v>25.274725274725274</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+        <v>106.82309362424954</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18">
         <f>SUM(C9:D11)</f>
         <v>91000000</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="6">
         <f>SUM(E9:E11)</f>
-        <v>99.999999999999986</v>
+        <v>422.64789216550901</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
@@ -1051,6 +1061,22 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:H12"/>
@@ -1062,22 +1088,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>